<commit_message>
minor changes to make design more flexible
</commit_message>
<xml_diff>
--- a/Ventilator_Interface_Board_RevA_BOM.xlsx
+++ b/Ventilator_Interface_Board_RevA_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="94">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -37,15 +37,28 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">2020-04-08</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2020-04-17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Fri 17 Apr 2020 17:21:26 BST</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Generated</t>
   </si>
   <si>
-    <t xml:space="preserve">Thu 09 Apr 2020 22:44:41 BST</t>
-  </si>
-  <si>
     <t xml:space="preserve">Company</t>
   </si>
   <si>
@@ -112,7 +125,7 @@
     <t xml:space="preserve">399-1099-1-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">C1 </t>
+    <t xml:space="preserve">C1 C7</t>
   </si>
   <si>
     <t xml:space="preserve">1uF</t>
@@ -127,82 +140,25 @@
     <t xml:space="preserve">311-1446-1-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">J4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LCD DISPLAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilator:Molex_KK-254_1x12_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Molex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22-05-3121 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WM4310-ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">J5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPTICAL SWITCH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilator:Molex_KK-254_1x05_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22-05-3051 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WM4303-ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">J6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOME LIMIT SWITCH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilator:Molex_KK-254_1x06_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22-05-3061 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WM4304-ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROTARY CONTROLS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilator:Molex_KK-254_1x08_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22-05-3081 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WM4306-ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">J3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALARM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilator:Molex_KK-254_1x04_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22-05-3041 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WM4302-ND </t>
+    <t xml:space="preserve">C8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1 J2 J3 J4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conn_01x08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventilator:PhoenixContact_PTSA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phoenix Contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">277-1628-ND</t>
   </si>
   <si>
     <t xml:space="preserve">P1 </t>
@@ -268,7 +224,7 @@
     <t xml:space="preserve">311-470HRCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">R8 R7 R1 </t>
+    <t xml:space="preserve">R8 R10 R1 </t>
   </si>
   <si>
     <t xml:space="preserve">330R</t>
@@ -280,7 +236,7 @@
     <t xml:space="preserve">311-330HRCT-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">R3 R2 </t>
+    <t xml:space="preserve">R2 R9</t>
   </si>
   <si>
     <t xml:space="preserve">10K</t>
@@ -292,6 +248,18 @@
     <t xml:space="preserve">311-10.0KHRCT-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">R3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0R</t>
+  </si>
+  <si>
     <t xml:space="preserve">SW1 </t>
   </si>
   <si>
@@ -319,28 +287,19 @@
     <t xml:space="preserve">U1 </t>
   </si>
   <si>
-    <t xml:space="preserve">HSCMRRN100MDAA5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilator:SMT-8W_7.5x8.8mm_P2.54mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Honeywell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSCMRRN100MDAA5-ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSCMRRN100MDAA5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Stock in Digikey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNF</t>
+    <t xml:space="preserve">MP3V5004GP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventilator:SOP_16.8x7.62mm_P2.54mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NXP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MP35004GP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MP3V5004GP-ND </t>
   </si>
   <si>
     <t xml:space="preserve">Green </t>
@@ -374,6 +333,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -391,7 +351,6 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -408,11 +367,13 @@
       <color rgb="FF009353"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
@@ -428,7 +389,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,12 +400,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCE181E"/>
-        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -498,7 +453,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -514,20 +469,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -551,7 +506,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -615,20 +570,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E:E"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="92.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
@@ -662,564 +617,488 @@
       <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="E16" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="F16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="H16" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="0" t="s">
+      <c r="D17" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="0" t="s">
+      <c r="F17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="5" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>35</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="B19" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="D19" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18" s="5" t="s">
+      <c r="F19" s="6" t="n">
+        <v>1985250</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>85</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="8" t="n">
+        <v>85</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>60</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="8" t="n">
         <v>85</v>
       </c>
-      <c r="G23" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>65</v>
+      <c r="G23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C24" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="8" t="n">
+        <v>85</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D27" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="6" t="n">
-        <v>85</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I24" s="6" t="s">
+      <c r="G27" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" s="5" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="6" t="n">
-        <v>85</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F27" s="6" t="n">
-        <v>85</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>81</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D29" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="B31" s="0" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B33" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="B32" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>106</v>
+      <c r="C32" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="s">
-        <v>107</v>
+      <c r="A36" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>